<commit_message>
Updated Examples & added Readme
Added the Newton's Method example
</commit_message>
<xml_diff>
--- a/example/example.xlsx
+++ b/example/example.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Documents\Projects\standalone-Formula.js\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Documents\sheetcalc.js\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Run Times</t>
   </si>
@@ -42,6 +43,15 @@
   </si>
   <si>
     <t>Low</t>
+  </si>
+  <si>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Equ</t>
+  </si>
+  <si>
+    <t>Equ`</t>
   </si>
 </sst>
 </file>
@@ -361,8 +371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,4 +483,53 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <f>A2^6 -A2^5-6*A2^4-A2^2+A2+10</f>
+        <v>839920</v>
+      </c>
+      <c r="C2">
+        <f>6*A2^5-5*A2^4-24*A2^3-2*A2+1</f>
+        <v>525981</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2-B2/C2</f>
+        <v>8.4031362349590566</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>